<commit_message>
excel com a classificao de tweets
</commit_message>
<xml_diff>
--- a/Projeto_1/mcdonalds.xlsx
+++ b/Projeto_1/mcdonalds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/Git/cdados/Projeto_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2174D5F4-19CD-9546-AB19-FD0C4C9FBABC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3A8724-F786-274A-BD16-9BCC41DE64D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1996,7 +1996,7 @@
   <dimension ref="A1:C301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B302" sqref="B302"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2016,6 +2016,9 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2" t="s">
         <v>482</v>
       </c>
@@ -2024,1140 +2027,1824 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="80" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" ht="192" x14ac:dyDescent="0.2">
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="192" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" ht="128" x14ac:dyDescent="0.2">
+      <c r="B134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="128" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+      <c r="B150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="80" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+      <c r="B160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="80" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="B211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="B222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>223</v>
+      </c>
+      <c r="B224">
+        <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>224</v>
       </c>
+      <c r="B225">
+        <v>1</v>
+      </c>
     </row>
     <row r="226" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>225</v>
       </c>
+      <c r="B226">
+        <v>0</v>
+      </c>
     </row>
     <row r="227" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>226</v>
       </c>
+      <c r="B227">
+        <v>0</v>
+      </c>
     </row>
     <row r="228" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>227</v>
       </c>
+      <c r="B228">
+        <v>0</v>
+      </c>
     </row>
     <row r="229" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>228</v>
       </c>
+      <c r="B229">
+        <v>0</v>
+      </c>
     </row>
     <row r="230" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>229</v>
+      </c>
+      <c r="B230">
+        <v>1</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -3957,7 +4644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="e">
         <f>mcdonalds_br por que tiraram o super mc do B28cardápio?</f>
         <v>#NAME?</v>

</xml_diff>

<commit_message>
Arrumei os nomes da classficacao no excel
</commit_message>
<xml_diff>
--- a/Projeto_1/mcdonalds.xlsx
+++ b/Projeto_1/mcdonalds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/Git/cdados/Projeto_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3A8724-F786-274A-BD16-9BCC41DE64D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD8B4A6-4F66-A541-A36E-F51FFC253AFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="482">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1579,16 +1579,7 @@
     <t>desisti de ir almoçar no mcdonalds porque esta sol, obrigada sol por preservar minha saude</t>
   </si>
   <si>
-    <t>0 = irrelevante</t>
-  </si>
-  <si>
-    <t>1 = relevante</t>
-  </si>
-  <si>
-    <t>0=irrelevante</t>
-  </si>
-  <si>
-    <t>1=relevante</t>
+    <t>Classificação</t>
   </si>
 </sst>
 </file>
@@ -1647,7 +1638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1655,6 +1646,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1993,10 +1985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:B301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2004,26 +1996,23 @@
     <col min="1" max="1" width="146.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="3" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2031,7 +2020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2039,7 +2028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2047,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2055,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2063,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2071,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -2079,7 +2068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -2087,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2095,7 +2084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -2103,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -2111,7 +2100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -2119,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -2127,7 +2116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -4422,10 +4411,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:B181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4433,26 +4422,23 @@
     <col min="1" max="1" width="173.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C1" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>302</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>303</v>
       </c>
@@ -4460,7 +4446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>304</v>
       </c>
@@ -4468,7 +4454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>305</v>
       </c>
@@ -4476,7 +4462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>306</v>
       </c>
@@ -4484,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>307</v>
       </c>
@@ -4492,7 +4478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>308</v>
       </c>
@@ -4500,7 +4486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>309</v>
       </c>
@@ -4508,7 +4494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>310</v>
       </c>
@@ -4516,7 +4502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>311</v>
       </c>
@@ -4524,7 +4510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>312</v>
       </c>
@@ -4532,7 +4518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>313</v>
       </c>
@@ -4540,7 +4526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>314</v>
       </c>
@@ -4548,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>315</v>
       </c>
@@ -4556,7 +4542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>316</v>
       </c>

</xml_diff>